<commit_message>
New code for paper revision
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\Documents\Programming\LiquidCrystals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\Documents\Programming\GolovatyLiquidCrystals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9D7021-DDD9-4B5F-BCC8-2B986BE7EDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575D8EEF-AE4C-4B4D-8789-640A146E92C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{2BAE82A8-45E9-43A7-9928-BE85A32412E7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Energy at t=0.8</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>|F - Fref|</t>
+  </si>
+  <si>
+    <t>Energy at t=0.1</t>
   </si>
 </sst>
 </file>
@@ -329,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -353,6 +356,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,31 +691,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0CD6B5-5C35-4658-9CFC-28FADEB464C2}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -719,7 +723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
@@ -733,7 +737,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>17</v>
@@ -742,12 +746,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>10</v>
       </c>
       <c r="B4" s="19">
-        <v>4.3505728147653397E-2</v>
+        <v>5.5277508705783802E-2</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>5</v>
@@ -756,100 +760,100 @@
         <v>10</v>
       </c>
       <c r="F4" s="19">
-        <v>-2.6259514114181599E-2</v>
+        <v>0.153066905474987</v>
       </c>
       <c r="G4" s="13">
         <f>ABS(F4-F$8)</f>
-        <v>9.7866523466539831E-4</v>
+        <v>2.7821723975652995E-2</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>20</v>
       </c>
       <c r="B5" s="9">
-        <v>1.5920850645684399E-2</v>
+        <v>1.3387753817850701E-2</v>
       </c>
       <c r="C5" s="4">
         <f>(LOG(B4)-LOG(B5))/(LOG(A5)-LOG(A4))</f>
-        <v>1.4502879441303032</v>
+        <v>2.0457786693444735</v>
       </c>
       <c r="E5" s="5">
         <v>20</v>
       </c>
       <c r="F5" s="9">
-        <v>-2.5609925613394698E-2</v>
+        <v>0.173677776602322</v>
       </c>
       <c r="G5" s="3">
         <f>ABS(F5-F$8)</f>
-        <v>3.2907673387849723E-4</v>
+        <v>7.210852848317989E-3</v>
       </c>
       <c r="H5" s="4">
         <f>(LOG(G4)-LOG(G5))/(LOG(E5)-LOG(E4))</f>
-        <v>1.5723914215799697</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.9479700130148416</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>40</v>
       </c>
       <c r="B6" s="9">
-        <v>3.5479528586196099E-3</v>
+        <v>3.3089979620469102E-3</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" ref="C6:C7" si="0">(LOG(B5)-LOG(B6))/(LOG(A6)-LOG(A5))</f>
-        <v>2.1658586747512745</v>
+        <v>2.0164476189951466</v>
       </c>
       <c r="E6" s="5">
         <v>40</v>
       </c>
       <c r="F6" s="9">
-        <v>-2.53547291394868E-2</v>
+        <v>0.17907953104893801</v>
       </c>
       <c r="G6" s="3">
         <f>ABS(F6-F$8)</f>
-        <v>7.3880259970598994E-5</v>
+        <v>1.8090984017019862E-3</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" ref="H6:H7" si="1">(LOG(G5)-LOG(G6))/(LOG(E6)-LOG(E5))</f>
-        <v>2.1551631817788679</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.9948990191154352</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>80</v>
       </c>
       <c r="B7" s="9">
-        <v>8.3939336887538902E-4</v>
+        <v>8.0630448057797399E-4</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>2.0795678695534816</v>
+        <v>2.0369977589204322</v>
       </c>
       <c r="E7" s="5">
         <v>80</v>
       </c>
       <c r="F7" s="9">
-        <v>-2.5298641409720001E-2</v>
+        <v>0.18044882360572001</v>
       </c>
       <c r="G7" s="3">
         <f>ABS(F7-F$8)</f>
-        <v>1.7792530203800117E-5</v>
+        <v>4.3980584491998265E-4</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="1"/>
-        <v>2.0539172578749469</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2.040332199613347</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E8" s="5">
         <v>400</v>
       </c>
       <c r="F8" s="9">
-        <v>-2.5280848879516201E-2</v>
+        <v>0.18088862945063999</v>
       </c>
       <c r="G8" s="2">
         <f>ABS(F8-F$8)</f>
@@ -857,12 +861,12 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>11</v>
       </c>
@@ -885,7 +889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>200</v>
       </c>
@@ -894,23 +898,23 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C12" s="11">
-        <v>4.2743568489002498E-6</v>
+        <v>4.2759255746980998E-6</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="21">
-        <v>-2.5416152980161401E-2</v>
+        <v>-2.5427564566334101E-2</v>
       </c>
       <c r="F12" s="13">
         <f>ABS(E12-E$17)</f>
-        <v>4.7071931350006757E-7</v>
+        <v>4.6998867610226203E-7</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>400</v>
       </c>
@@ -919,25 +923,25 @@
         <v>2E-3</v>
       </c>
       <c r="C13" s="7">
-        <v>1.0684224227400999E-6</v>
+        <v>1.06881441369226E-6</v>
       </c>
       <c r="D13" s="8">
         <f>(LOG(C12)-LOG(C13))/(LOG(A13)-LOG(A12))</f>
-        <v>2.000225198926743</v>
+        <v>2.0002253734355739</v>
       </c>
       <c r="E13" s="22">
-        <v>-2.5415799928731799E-2</v>
+        <v>-2.5427212062880501E-2</v>
       </c>
       <c r="F13" s="3">
         <f>ABS(E13-E$17)</f>
-        <v>1.1766788389835914E-7</v>
+        <v>1.1748522250193405E-7</v>
       </c>
       <c r="G13" s="4">
         <f>(LOG(F12)-LOG(F13))/(LOG(A13)-LOG(A12))</f>
-        <v>2.0001464406608296</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2.0001466934633019</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>800</v>
       </c>
@@ -946,25 +950,25 @@
         <v>1E-3</v>
       </c>
       <c r="C14" s="7">
-        <v>2.6708441986148298E-7</v>
+        <v>2.6718239815483E-7</v>
       </c>
       <c r="D14" s="8">
         <f>(LOG(C13)-LOG(C14))/(LOG(A14)-LOG(A13))</f>
-        <v>2.0001144337449794</v>
+        <v>2.0001144967691862</v>
       </c>
       <c r="E14" s="22">
-        <v>-2.5415711676013801E-2</v>
+        <v>-2.54271239471488E-2</v>
       </c>
       <c r="F14" s="3">
         <f>ABS(E14-E$17)</f>
-        <v>2.9415165900270601E-8</v>
+        <v>2.9369490801151032E-8</v>
       </c>
       <c r="G14" s="4">
         <f>(LOG(F13)-LOG(F14))/(LOG(A14)-LOG(A13))</f>
-        <v>2.0000885288860109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2.0000891454738299</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>1600</v>
       </c>
@@ -973,25 +977,25 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="C15" s="7">
-        <v>6.6770986852458602E-8</v>
+        <v>6.6795472854015002E-8</v>
       </c>
       <c r="D15" s="8">
         <f>(LOG(C14)-LOG(C15))/(LOG(A15)-LOG(A14))</f>
-        <v>2.0000025520180285</v>
+        <v>2.0000027362214317</v>
       </c>
       <c r="E15" s="22">
-        <v>-2.5415689614906999E-2</v>
+        <v>-2.5427101920295101E-2</v>
       </c>
       <c r="F15" s="3">
         <f>ABS(E15-E$17)</f>
-        <v>7.3540590977971831E-9</v>
+        <v>7.3426371025031578E-9</v>
       </c>
       <c r="G15" s="4">
         <f>(LOG(F14)-LOG(F15))/(LOG(A15)-LOG(A14))</f>
-        <v>1.9999474977009237</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.9999480488239232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>3200</v>
       </c>
@@ -1000,25 +1004,29 @@
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="C16" s="7">
-        <v>1.6684127657344299E-8</v>
+        <v>1.6690242116144301E-8</v>
       </c>
       <c r="D16" s="8">
         <f>(LOG(C15)-LOG(C16))/(LOG(A16)-LOG(A15))</f>
-        <v>2.0007451068758217</v>
+        <v>2.0007454423335456</v>
       </c>
       <c r="E16" s="22">
-        <v>-2.5415684098535299E-2</v>
+        <v>-2.5427096412487801E-2</v>
       </c>
       <c r="F16" s="3">
         <f>ABS(E16-E$17)</f>
-        <v>1.8376873980874286E-9</v>
+        <v>1.8348298019832399E-9</v>
       </c>
       <c r="G16" s="4">
         <f>(LOG(F15)-LOG(F16))/(LOG(A16)-LOG(A15))</f>
-        <v>2.0006493939877896</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2.0006520534488601</v>
+      </c>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>80000</v>
       </c>
@@ -1029,19 +1037,33 @@
       <c r="C17" s="6"/>
       <c r="D17" s="5"/>
       <c r="E17" s="22">
-        <v>-2.5415682260847901E-2</v>
+        <v>-2.5427094577657999E-2</v>
       </c>
       <c r="F17" s="2">
         <v>0</v>
       </c>
       <c r="G17" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+    </row>
+    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>7</v>
       </c>
@@ -1060,8 +1082,12 @@
       <c r="F20" s="14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>10</v>
       </c>
@@ -1070,10 +1096,10 @@
         <v>0.2</v>
       </c>
       <c r="C21" s="19">
-        <v>7.9800939559936501E-2</v>
+        <v>7.9777383804321297E-2</v>
       </c>
       <c r="D21" s="13">
-        <v>7.9800987243652297E-2</v>
+        <v>7.9777431488037107E-2</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>5</v>
@@ -1081,8 +1107,10 @@
       <c r="F21" s="10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K21" s="23"/>
+      <c r="N21" s="23"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -1091,21 +1119,21 @@
         <v>0.1</v>
       </c>
       <c r="C22" s="9">
-        <v>2.2379477968934199E-2</v>
+        <v>2.23781786571066E-2</v>
       </c>
       <c r="D22" s="3">
-        <v>2.23794969949608E-2</v>
+        <v>2.23781976775171E-2</v>
       </c>
       <c r="E22" s="4">
         <f>(LOG(C22)-LOG(C21))/(LOG(B22)-LOG(B21))</f>
-        <v>1.8342293486162395</v>
+        <v>1.8338871916475241</v>
       </c>
       <c r="F22" s="4">
         <f>(LOG(D22)-LOG(D21))/(LOG(B22)-LOG(B21))</f>
-        <v>1.8342289841602781</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.8338868277369518</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>40</v>
       </c>
@@ -1114,21 +1142,21 @@
         <v>0.05</v>
       </c>
       <c r="C23" s="9">
-        <v>7.7537296564120497E-3</v>
+        <v>7.7581453496418399E-3</v>
       </c>
       <c r="D23" s="3">
-        <v>7.7537349920953902E-3</v>
+        <v>7.7581506850154004E-3</v>
       </c>
       <c r="E23" s="4">
         <f>(LOG(C23)-LOG(C22))/(LOG(B23)-LOG(B22))</f>
-        <v>1.5292140442356985</v>
+        <v>1.528308910969927</v>
       </c>
       <c r="F23" s="4">
         <f t="shared" ref="F23:F26" si="4">(LOG(D23)-LOG(D22))/(LOG(B23)-LOG(B22))</f>
-        <v>1.5292142779679334</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.5283091450339796</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>80</v>
       </c>
@@ -1137,21 +1165,21 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C24" s="9">
-        <v>2.0004965767757002E-3</v>
+        <v>1.9887971747154501E-3</v>
       </c>
       <c r="D24" s="3">
-        <v>2.0004984254089102E-3</v>
+        <v>1.9887990244014399E-3</v>
       </c>
       <c r="E24" s="4">
         <f>(LOG(C24)-LOG(C23))/(LOG(B24)-LOG(B23))</f>
-        <v>1.9545322746150808</v>
+        <v>1.9638156531483482</v>
       </c>
       <c r="F24" s="4">
         <f t="shared" si="4"/>
-        <v>1.9545319342214711</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.9638153035257684</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>160</v>
       </c>
@@ -1160,21 +1188,21 @@
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="C25" s="9">
-        <v>4.0706868526231999E-4</v>
+        <v>4.0725399661228402E-4</v>
       </c>
       <c r="D25" s="3">
-        <v>4.0706892374009598E-4</v>
+        <v>4.0725423369538202E-4</v>
       </c>
       <c r="E25" s="4">
         <f>(LOG(C25)-LOG(C24))/(LOG(B25)-LOG(B24))</f>
-        <v>2.2970140118910063</v>
+        <v>2.2878953901025212</v>
       </c>
       <c r="F25" s="4">
         <f t="shared" si="4"/>
-        <v>2.2970144998758153</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2.287895892018851</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>320</v>
       </c>
@@ -1183,21 +1211,22 @@
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="C26" s="9">
-        <v>9.1600605900368402E-5</v>
+        <v>9.1693572748853503E-5</v>
       </c>
       <c r="D26" s="3">
-        <v>9.1600654426737197E-5</v>
+        <v>9.1693621297313094E-5</v>
       </c>
       <c r="E26" s="4">
         <f>(LOG(C26)-LOG(C25))/(LOG(B26)-LOG(B25))</f>
-        <v>2.1518431966592826</v>
+        <v>2.1510363398744259</v>
       </c>
       <c r="F26" s="4">
         <f t="shared" si="4"/>
-        <v>2.1518432775674032</v>
+        <v>2.1510364158846493</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>